<commit_message>
changes frontend page names and column names based on excel
</commit_message>
<xml_diff>
--- a/transfer_by_CommArts_history.xlsx
+++ b/transfer_by_CommArts_history.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="166">
   <si>
     <t xml:space="preserve">State Name</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t xml:space="preserve">COM 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNHM Course #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNHM Course Title</t>
   </si>
   <si>
     <t xml:space="preserve">Expires </t>
@@ -1467,7 +1479,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1491,10 +1503,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>3</v>
@@ -1503,10 +1515,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>7</v>
@@ -1515,7 +1527,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>10</v>
@@ -1526,26 +1538,26 @@
         <v>57</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J2" s="17"/>
       <c r="K2" s="7"/>
@@ -1555,13 +1567,13 @@
         <v>57</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>21</v>
@@ -1574,7 +1586,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="20"/>
@@ -1584,13 +1596,13 @@
         <v>57</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>21</v>
@@ -1603,7 +1615,7 @@
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="20"/>
@@ -1613,26 +1625,26 @@
         <v>57</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="10"/>
@@ -1642,13 +1654,13 @@
         <v>57</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>21</v>
@@ -1661,7 +1673,7 @@
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="10"/>
@@ -1671,26 +1683,26 @@
         <v>57</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="10"/>
@@ -1700,26 +1712,26 @@
         <v>57</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="10"/>
@@ -1729,13 +1741,13 @@
         <v>57</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>21</v>
@@ -1748,7 +1760,7 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="10"/>
@@ -1758,13 +1770,13 @@
         <v>57</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>21</v>
@@ -1777,7 +1789,7 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="10"/>
@@ -1787,26 +1799,26 @@
         <v>57</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="10"/>
@@ -1816,26 +1828,26 @@
         <v>57</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="10"/>
@@ -1845,26 +1857,26 @@
         <v>57</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="10"/>
@@ -1874,26 +1886,26 @@
         <v>57</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="10"/>
@@ -1903,26 +1915,26 @@
         <v>57</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="10"/>
@@ -1935,23 +1947,23 @@
         <v>75</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="10"/>
@@ -1964,10 +1976,10 @@
         <v>75</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>21</v>
@@ -1980,7 +1992,7 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="10"/>
@@ -1993,10 +2005,10 @@
         <v>75</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>21</v>
@@ -2009,7 +2021,7 @@
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="20"/>
@@ -2022,10 +2034,10 @@
         <v>75</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>21</v>
@@ -2038,7 +2050,7 @@
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="10"/>
@@ -2051,23 +2063,23 @@
         <v>75</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="10"/>
@@ -2080,23 +2092,23 @@
         <v>75</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="20"/>
@@ -2109,10 +2121,10 @@
         <v>75</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>21</v>
@@ -2125,7 +2137,7 @@
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="20"/>
@@ -2138,23 +2150,23 @@
         <v>75</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="20"/>
@@ -2167,23 +2179,23 @@
         <v>75</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="10"/>
@@ -2196,23 +2208,23 @@
         <v>75</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="20"/>
@@ -2225,23 +2237,23 @@
         <v>75</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="10"/>
@@ -2254,23 +2266,23 @@
         <v>75</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="10"/>
@@ -2283,23 +2295,23 @@
         <v>75</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="10"/>

</xml_diff>